<commit_message>
cleaning, ready color comparison
</commit_message>
<xml_diff>
--- a/masks+pic/comparison_color.xlsx
+++ b/masks+pic/comparison_color.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b95324ec1dbd516d/Dokumenty/GitHub/G/masks^Mpic/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="172" documentId="8_{E4594A22-AFE3-454B-A66C-71E7CD8BEF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A4A5855-04EE-49F1-8D4A-B84412B91EA6}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{E4594A22-AFE3-454B-A66C-71E7CD8BEF9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4527EBE6-179D-4000-9CE7-91E242304811}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{8DDA7121-79A4-441C-B316-0237A835ED06}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11175" xr2:uid="{8DDA7121-79A4-441C-B316-0237A835ED06}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -521,12 +521,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -541,7 +547,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -550,6 +556,7 @@
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -565,6 +572,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -886,21 +897,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D519F41-A112-4A68-AC6F-405E518203B9}">
   <dimension ref="A1:J123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6328125" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.1796875" customWidth="1"/>
-    <col min="6" max="6" width="8.7265625" style="3"/>
-    <col min="9" max="9" width="9.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" style="3"/>
+    <col min="9" max="9" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>122</v>
       </c>
@@ -932,11 +943,11 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="4">
         <v>2</v>
       </c>
       <c r="D2" s="3">
@@ -951,19 +962,22 @@
       <c r="G2" s="3">
         <v>2</v>
       </c>
+      <c r="H2" s="3">
+        <v>2</v>
+      </c>
       <c r="I2" s="3">
-        <f>GEOMEAN(D2:G2)</f>
+        <f>GEOMEAN(D2:H2)</f>
         <v>2</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
       <c r="D3" s="3">
@@ -978,17 +992,20 @@
       <c r="G3" s="3">
         <v>2</v>
       </c>
+      <c r="H3" s="3">
+        <v>2</v>
+      </c>
       <c r="I3" s="3">
-        <f t="shared" ref="I3:I66" si="0">GEOMEAN(D3:G3)</f>
+        <f t="shared" ref="I3:I66" si="0">GEOMEAN(D3:H3)</f>
         <v>2</v>
       </c>
       <c r="J3" s="2"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="4">
         <v>2</v>
       </c>
       <c r="D4" s="3">
@@ -1003,19 +1020,22 @@
       <c r="G4" s="3">
         <v>1</v>
       </c>
+      <c r="H4" s="3">
+        <v>3</v>
+      </c>
       <c r="I4" s="3">
         <f t="shared" si="0"/>
-        <v>1.8612097182041991</v>
+        <v>2.0476725110792193</v>
       </c>
       <c r="J4" s="1" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
       <c r="D5" s="3">
@@ -1030,17 +1050,20 @@
       <c r="G5" s="3">
         <v>2</v>
       </c>
+      <c r="H5" s="3">
+        <v>2</v>
+      </c>
       <c r="I5" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="J5" s="2"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
       <c r="D6" s="3">
@@ -1055,15 +1078,18 @@
       <c r="G6" s="3">
         <v>2</v>
       </c>
+      <c r="H6" s="3">
+        <v>2</v>
+      </c>
       <c r="I6" s="3">
         <f t="shared" si="0"/>
-        <v>1.681792830507429</v>
+        <v>1.7411011265922482</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1082,17 +1108,20 @@
       <c r="G7" s="3">
         <v>2</v>
       </c>
+      <c r="H7" s="3">
+        <v>1</v>
+      </c>
       <c r="I7" s="3">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1.7411011265922482</v>
       </c>
       <c r="J7" s="2"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="4">
         <v>1</v>
       </c>
       <c r="D8" s="3">
@@ -1107,15 +1136,18 @@
       <c r="G8" s="3">
         <v>2</v>
       </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
       <c r="I8" s="3">
         <f t="shared" si="0"/>
-        <v>1.189207115002721</v>
+        <v>1.1486983549970351</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1134,12 +1166,15 @@
       <c r="G9" s="3">
         <v>2</v>
       </c>
+      <c r="H9" s="3">
+        <v>1</v>
+      </c>
       <c r="I9" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1158,16 +1193,19 @@
       <c r="G10" s="3">
         <v>2</v>
       </c>
+      <c r="H10" s="3">
+        <v>2</v>
+      </c>
       <c r="I10" s="3">
         <f t="shared" si="0"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="4">
         <v>2</v>
       </c>
       <c r="D11" s="3">
@@ -1182,12 +1220,15 @@
       <c r="G11" s="3">
         <v>2</v>
       </c>
+      <c r="H11" s="3">
+        <v>3</v>
+      </c>
       <c r="I11" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>2.3521580450493471</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1206,16 +1247,19 @@
       <c r="G12" s="3">
         <v>2</v>
       </c>
+      <c r="H12" s="3">
+        <v>2</v>
+      </c>
       <c r="I12" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="4">
         <v>2</v>
       </c>
       <c r="D13" s="3">
@@ -1230,16 +1274,19 @@
       <c r="G13" s="3">
         <v>3</v>
       </c>
+      <c r="H13" s="3">
+        <v>2</v>
+      </c>
       <c r="I13" s="3">
         <f t="shared" si="0"/>
-        <v>2.5900200641113513</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>2.4595094858493631</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="4">
         <v>2</v>
       </c>
       <c r="D14" s="3">
@@ -1254,16 +1301,19 @@
       <c r="G14" s="3">
         <v>1</v>
       </c>
+      <c r="H14" s="3">
+        <v>2</v>
+      </c>
       <c r="I14" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="4">
         <v>2</v>
       </c>
       <c r="D15" s="3">
@@ -1278,12 +1328,15 @@
       <c r="G15" s="3">
         <v>2</v>
       </c>
+      <c r="H15" s="3">
+        <v>1</v>
+      </c>
       <c r="I15" s="3">
         <f t="shared" si="0"/>
-        <v>1.681792830507429</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1302,16 +1355,19 @@
       <c r="G16" s="3">
         <v>3</v>
       </c>
+      <c r="H16" s="3">
+        <v>3</v>
+      </c>
       <c r="I16" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.3521580450493471</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="4">
         <v>1</v>
       </c>
       <c r="D17" s="3">
@@ -1326,12 +1382,15 @@
       <c r="G17" s="3">
         <v>1</v>
       </c>
+      <c r="H17" s="3">
+        <v>1</v>
+      </c>
       <c r="I17" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1350,16 +1409,19 @@
       <c r="G18" s="3">
         <v>4</v>
       </c>
+      <c r="H18" s="3">
+        <v>3</v>
+      </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
-        <v>3.2237097954706257</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.177671523146437</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="4">
         <v>2</v>
       </c>
       <c r="D19" s="3">
@@ -1374,16 +1436,19 @@
       <c r="G19" s="3">
         <v>3</v>
       </c>
+      <c r="H19" s="3">
+        <v>2</v>
+      </c>
       <c r="I19" s="3">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.3521580450493471</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="4">
         <v>2</v>
       </c>
       <c r="D20" s="3">
@@ -1398,12 +1463,15 @@
       <c r="G20" s="3">
         <v>3</v>
       </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
       <c r="I20" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1422,16 +1490,19 @@
       <c r="G21" s="3">
         <v>2</v>
       </c>
+      <c r="H21" s="3">
+        <v>1</v>
+      </c>
       <c r="I21" s="3">
         <f t="shared" si="0"/>
-        <v>1.681792830507429</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="4">
         <v>2</v>
       </c>
       <c r="D22" s="3">
@@ -1446,16 +1517,19 @@
       <c r="G22" s="3">
         <v>3</v>
       </c>
+      <c r="H22" s="3">
+        <v>1</v>
+      </c>
       <c r="I22" s="3">
         <f t="shared" si="0"/>
-        <v>2.340347319320716</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.97435048583482</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="4">
         <v>2</v>
       </c>
       <c r="D23" s="3">
@@ -1470,16 +1544,19 @@
       <c r="G23" s="3">
         <v>2</v>
       </c>
+      <c r="H23" s="3">
+        <v>2</v>
+      </c>
       <c r="I23" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="4">
         <v>2</v>
       </c>
       <c r="D24" s="3">
@@ -1494,16 +1571,19 @@
       <c r="G24" s="3">
         <v>2</v>
       </c>
+      <c r="H24" s="3">
+        <v>2</v>
+      </c>
       <c r="I24" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="4">
         <v>2</v>
       </c>
       <c r="D25" s="3">
@@ -1518,12 +1598,15 @@
       <c r="G25" s="3">
         <v>3</v>
       </c>
+      <c r="H25" s="3">
+        <v>2</v>
+      </c>
       <c r="I25" s="3">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.3521580450493471</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1542,12 +1625,15 @@
       <c r="G26" s="3">
         <v>2</v>
       </c>
+      <c r="H26" s="3">
+        <v>3</v>
+      </c>
       <c r="I26" s="3">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.5508490012515819</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1566,16 +1652,19 @@
       <c r="G27" s="3">
         <v>2</v>
       </c>
+      <c r="H27" s="3">
+        <v>2</v>
+      </c>
       <c r="I27" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="4">
         <v>1</v>
       </c>
       <c r="D28" s="3">
@@ -1590,16 +1679,19 @@
       <c r="G28" s="3">
         <v>2</v>
       </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
       <c r="I28" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="4">
         <v>2</v>
       </c>
       <c r="D29" s="3">
@@ -1614,12 +1706,15 @@
       <c r="G29" s="3">
         <v>3</v>
       </c>
+      <c r="H29" s="3">
+        <v>1</v>
+      </c>
       <c r="I29" s="3">
         <f t="shared" si="0"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1638,16 +1733,19 @@
       <c r="G30" s="3">
         <v>2</v>
       </c>
+      <c r="H30" s="3">
+        <v>2</v>
+      </c>
       <c r="I30" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="4">
         <v>1</v>
       </c>
       <c r="D31" s="3">
@@ -1662,12 +1760,15 @@
       <c r="G31" s="3">
         <v>2</v>
       </c>
+      <c r="H31" s="3">
+        <v>1</v>
+      </c>
       <c r="I31" s="3">
         <f t="shared" si="0"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1686,16 +1787,19 @@
       <c r="G32" s="3">
         <v>3</v>
       </c>
+      <c r="H32" s="3">
+        <v>2</v>
+      </c>
       <c r="I32" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="4">
         <v>2</v>
       </c>
       <c r="D33" s="3">
@@ -1710,12 +1814,15 @@
       <c r="G33" s="3">
         <v>3</v>
       </c>
+      <c r="H33" s="3">
+        <v>2</v>
+      </c>
       <c r="I33" s="3">
         <f t="shared" si="0"/>
-        <v>2.340347319320716</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.2679331552660544</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1734,12 +1841,15 @@
       <c r="G34" s="3">
         <v>4</v>
       </c>
+      <c r="H34" s="3">
+        <v>3</v>
+      </c>
       <c r="I34" s="3">
         <f t="shared" si="0"/>
-        <v>2.6321480259049852</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7019200770412271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1758,16 +1868,19 @@
       <c r="G35" s="3">
         <v>2</v>
       </c>
+      <c r="H35" s="3">
+        <v>3</v>
+      </c>
       <c r="I35" s="3">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.5508490012515819</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="4">
         <v>2</v>
       </c>
       <c r="D36" s="3">
@@ -1782,16 +1895,19 @@
       <c r="G36" s="3">
         <v>2</v>
       </c>
+      <c r="H36" s="3">
+        <v>2</v>
+      </c>
       <c r="I36" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="4">
         <v>2</v>
       </c>
       <c r="D37" s="3">
@@ -1806,16 +1922,19 @@
       <c r="G37" s="3">
         <v>2</v>
       </c>
+      <c r="H37" s="3">
+        <v>2</v>
+      </c>
       <c r="I37" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="4">
         <v>2</v>
       </c>
       <c r="D38" s="3">
@@ -1830,16 +1949,19 @@
       <c r="G38" s="3">
         <v>3</v>
       </c>
+      <c r="H38" s="3">
+        <v>2</v>
+      </c>
       <c r="I38" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="4">
         <v>2</v>
       </c>
       <c r="D39" s="3">
@@ -1854,16 +1976,19 @@
       <c r="G39" s="3">
         <v>3</v>
       </c>
+      <c r="H39" s="3">
+        <v>2</v>
+      </c>
       <c r="I39" s="3">
         <f t="shared" si="0"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="4">
         <v>2</v>
       </c>
       <c r="D40" s="3">
@@ -1878,16 +2003,19 @@
       <c r="G40" s="3">
         <v>3</v>
       </c>
+      <c r="H40" s="3">
+        <v>1</v>
+      </c>
       <c r="I40" s="3">
         <f t="shared" si="0"/>
-        <v>1.7320508075688774</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.5518455739153598</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="4">
         <v>3</v>
       </c>
       <c r="D41" s="3">
@@ -1902,16 +2030,19 @@
       <c r="G41" s="3">
         <v>3</v>
       </c>
+      <c r="H41" s="3">
+        <v>3</v>
+      </c>
       <c r="I41" s="3">
         <f t="shared" si="0"/>
-        <v>2.4494897427831779</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.5508490012515819</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="4">
         <v>2</v>
       </c>
       <c r="D42" s="3">
@@ -1926,12 +2057,15 @@
       <c r="G42" s="3">
         <v>2</v>
       </c>
+      <c r="H42" s="3">
+        <v>2</v>
+      </c>
       <c r="I42" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -1950,16 +2084,19 @@
       <c r="G43" s="3">
         <v>3</v>
       </c>
+      <c r="H43" s="3">
+        <v>3</v>
+      </c>
       <c r="I43" s="3">
         <f t="shared" si="0"/>
-        <v>2.7108060108295344</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7663237344451832</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="4">
         <v>2</v>
       </c>
       <c r="D44" s="3">
@@ -1974,12 +2111,15 @@
       <c r="G44" s="3">
         <v>2</v>
       </c>
+      <c r="H44" s="3">
+        <v>2</v>
+      </c>
       <c r="I44" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -1998,12 +2138,15 @@
       <c r="G45" s="3">
         <v>1</v>
       </c>
+      <c r="H45" s="3">
+        <v>1</v>
+      </c>
       <c r="I45" s="3">
         <f t="shared" si="0"/>
-        <v>1.1066819197003217</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.0844717711976986</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2022,12 +2165,15 @@
       <c r="G46" s="3">
         <v>2</v>
       </c>
+      <c r="H46" s="3">
+        <v>1</v>
+      </c>
       <c r="I46" s="3">
         <f t="shared" si="0"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2046,16 +2192,19 @@
       <c r="G47" s="3">
         <v>2</v>
       </c>
+      <c r="H47" s="3">
+        <v>2</v>
+      </c>
       <c r="I47" s="3">
         <f t="shared" si="0"/>
-        <v>2.1147425268811282</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.0912791051825463</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="4">
         <v>3</v>
       </c>
       <c r="D48" s="3">
@@ -2070,12 +2219,15 @@
       <c r="G48" s="3">
         <v>3</v>
       </c>
+      <c r="H48" s="3">
+        <v>3</v>
+      </c>
       <c r="I48" s="3">
         <f t="shared" si="0"/>
-        <v>3.3503689588345078</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+        <v>3.2771653924211188</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2094,16 +2246,19 @@
       <c r="G49" s="3">
         <v>1</v>
       </c>
+      <c r="H49" s="3">
+        <v>2</v>
+      </c>
       <c r="I49" s="3">
         <f t="shared" si="0"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="4">
         <v>2</v>
       </c>
       <c r="D50" s="3">
@@ -2118,16 +2273,19 @@
       <c r="G50" s="3">
         <v>2</v>
       </c>
+      <c r="H50" s="3">
+        <v>2</v>
+      </c>
       <c r="I50" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="4">
         <v>2</v>
       </c>
       <c r="D51" s="3">
@@ -2142,16 +2300,19 @@
       <c r="G51" s="3">
         <v>3</v>
       </c>
+      <c r="H51" s="3">
+        <v>2</v>
+      </c>
       <c r="I51" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="4">
         <v>2</v>
       </c>
       <c r="D52" s="3">
@@ -2166,12 +2327,15 @@
       <c r="G52" s="3">
         <v>2</v>
       </c>
+      <c r="H52" s="3">
+        <v>2</v>
+      </c>
       <c r="I52" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2190,12 +2354,15 @@
       <c r="G53" s="3">
         <v>3</v>
       </c>
+      <c r="H53" s="3">
+        <v>2</v>
+      </c>
       <c r="I53" s="3">
         <f t="shared" si="0"/>
-        <v>2.7108060108295344</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.5508490012515819</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2214,16 +2381,19 @@
       <c r="G54" s="3">
         <v>2</v>
       </c>
+      <c r="H54" s="3">
+        <v>1</v>
+      </c>
       <c r="I54" s="3">
         <f t="shared" si="0"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4309690811052556</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
-      <c r="B55">
+      <c r="B55" s="4">
         <v>2</v>
       </c>
       <c r="D55" s="3">
@@ -2238,16 +2408,19 @@
       <c r="G55" s="3">
         <v>3</v>
       </c>
+      <c r="H55" s="3">
+        <v>2</v>
+      </c>
       <c r="I55" s="3">
         <f t="shared" si="0"/>
-        <v>2.5900200641113513</v>
-      </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.4595094858493631</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B56">
+      <c r="B56" s="4">
         <v>2</v>
       </c>
       <c r="D56" s="3">
@@ -2262,16 +2435,19 @@
       <c r="G56" s="3">
         <v>2</v>
       </c>
+      <c r="H56" s="3">
+        <v>2</v>
+      </c>
       <c r="I56" s="3">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
-      <c r="B57">
+      <c r="B57" s="4">
         <v>2</v>
       </c>
       <c r="D57" s="3">
@@ -2286,16 +2462,19 @@
       <c r="G57" s="3">
         <v>3</v>
       </c>
+      <c r="H57" s="3">
+        <v>2</v>
+      </c>
       <c r="I57" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
-      <c r="B58">
+      <c r="B58" s="4">
         <v>2</v>
       </c>
       <c r="D58" s="3">
@@ -2310,12 +2489,15 @@
       <c r="G58" s="3">
         <v>2</v>
       </c>
+      <c r="H58" s="3">
+        <v>2</v>
+      </c>
       <c r="I58" s="3">
         <f t="shared" si="0"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2334,16 +2516,19 @@
       <c r="G59" s="3">
         <v>3</v>
       </c>
+      <c r="H59" s="3">
+        <v>3</v>
+      </c>
       <c r="I59" s="3">
         <f t="shared" si="0"/>
-        <v>2.9129506302439405</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.9301560515835217</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="B60">
+      <c r="B60" s="4">
         <v>2</v>
       </c>
       <c r="D60" s="3">
@@ -2358,16 +2543,19 @@
       <c r="G60" s="3">
         <v>3</v>
       </c>
+      <c r="H60" s="3">
+        <v>2</v>
+      </c>
       <c r="I60" s="3">
         <f t="shared" si="0"/>
-        <v>2.5900200641113513</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.4595094858493631</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
-      <c r="B61">
+      <c r="B61" s="4">
         <v>2</v>
       </c>
       <c r="D61" s="3">
@@ -2382,12 +2570,15 @@
       <c r="G61" s="3">
         <v>2</v>
       </c>
+      <c r="H61" s="3">
+        <v>2</v>
+      </c>
       <c r="I61" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2406,12 +2597,15 @@
       <c r="G62" s="3">
         <v>3</v>
       </c>
+      <c r="H62" s="3">
+        <v>2</v>
+      </c>
       <c r="I62" s="3">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7663237344451832</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2430,12 +2624,15 @@
       <c r="G63" s="3">
         <v>1</v>
       </c>
+      <c r="H63" s="3">
+        <v>1</v>
+      </c>
       <c r="I63" s="3">
         <f t="shared" si="0"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -2454,16 +2651,19 @@
       <c r="G64" s="3">
         <v>3</v>
       </c>
+      <c r="H64" s="3">
+        <v>2</v>
+      </c>
       <c r="I64" s="3">
         <f t="shared" si="0"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>63</v>
       </c>
-      <c r="B65">
+      <c r="B65" s="4">
         <v>2</v>
       </c>
       <c r="D65" s="3">
@@ -2478,16 +2678,19 @@
       <c r="G65" s="3">
         <v>3</v>
       </c>
+      <c r="H65" s="3">
+        <v>2</v>
+      </c>
       <c r="I65" s="3">
         <f t="shared" si="0"/>
-        <v>2.340347319320716</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.2679331552660544</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>64</v>
       </c>
-      <c r="B66">
+      <c r="B66" s="4">
         <v>1</v>
       </c>
       <c r="D66" s="3">
@@ -2502,16 +2705,19 @@
       <c r="G66" s="3">
         <v>2</v>
       </c>
+      <c r="H66" s="3">
+        <v>1</v>
+      </c>
       <c r="I66" s="3">
         <f t="shared" si="0"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>65</v>
       </c>
-      <c r="B67">
+      <c r="B67" s="4">
         <v>2</v>
       </c>
       <c r="D67" s="3">
@@ -2526,12 +2732,15 @@
       <c r="G67" s="3">
         <v>3</v>
       </c>
+      <c r="H67" s="3">
+        <v>2</v>
+      </c>
       <c r="I67" s="3">
-        <f t="shared" ref="I67:I123" si="1">GEOMEAN(D67:G67)</f>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+        <f t="shared" ref="I67:I123" si="1">GEOMEAN(D67:H67)</f>
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>66</v>
       </c>
@@ -2550,16 +2759,19 @@
       <c r="G68" s="3">
         <v>1</v>
       </c>
+      <c r="H68" s="3">
+        <v>2</v>
+      </c>
       <c r="I68" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>67</v>
       </c>
-      <c r="B69">
+      <c r="B69" s="4">
         <v>2</v>
       </c>
       <c r="D69" s="3">
@@ -2574,12 +2786,15 @@
       <c r="G69" s="3">
         <v>2</v>
       </c>
+      <c r="H69" s="3">
+        <v>2</v>
+      </c>
       <c r="I69" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>68</v>
       </c>
@@ -2598,12 +2813,15 @@
       <c r="G70" s="3">
         <v>1</v>
       </c>
+      <c r="H70" s="3">
+        <v>1</v>
+      </c>
       <c r="I70" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>69</v>
       </c>
@@ -2622,16 +2840,19 @@
       <c r="G71" s="3">
         <v>1</v>
       </c>
+      <c r="H71" s="3">
+        <v>1</v>
+      </c>
       <c r="I71" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>70</v>
       </c>
-      <c r="B72">
+      <c r="B72" s="4">
         <v>2</v>
       </c>
       <c r="D72" s="3">
@@ -2646,16 +2867,19 @@
       <c r="G72" s="3">
         <v>2</v>
       </c>
+      <c r="H72" s="3">
+        <v>2</v>
+      </c>
       <c r="I72" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>71</v>
       </c>
-      <c r="B73">
+      <c r="B73" s="4">
         <v>2</v>
       </c>
       <c r="D73" s="3">
@@ -2670,16 +2894,19 @@
       <c r="G73" s="3">
         <v>1</v>
       </c>
+      <c r="H73" s="3">
+        <v>2</v>
+      </c>
       <c r="I73" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>72</v>
       </c>
-      <c r="B74">
+      <c r="B74" s="4">
         <v>2</v>
       </c>
       <c r="D74" s="3">
@@ -2694,16 +2921,19 @@
       <c r="G74" s="3">
         <v>2</v>
       </c>
+      <c r="H74" s="3">
+        <v>2</v>
+      </c>
       <c r="I74" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>73</v>
       </c>
-      <c r="B75">
+      <c r="B75" s="4">
         <v>2</v>
       </c>
       <c r="D75" s="3">
@@ -2718,16 +2948,19 @@
       <c r="G75" s="3">
         <v>2</v>
       </c>
+      <c r="H75" s="3">
+        <v>2</v>
+      </c>
       <c r="I75" s="3">
         <f t="shared" si="1"/>
-        <v>2.1147425268811282</v>
-      </c>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.0912791051825463</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>74</v>
       </c>
-      <c r="B76">
+      <c r="B76" s="4">
         <v>2</v>
       </c>
       <c r="D76" s="3">
@@ -2742,12 +2975,15 @@
       <c r="G76" s="3">
         <v>1</v>
       </c>
+      <c r="H76" s="3">
+        <v>2</v>
+      </c>
       <c r="I76" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>75</v>
       </c>
@@ -2766,12 +3002,15 @@
       <c r="G77" s="3">
         <v>2</v>
       </c>
+      <c r="H77" s="3">
+        <v>1</v>
+      </c>
       <c r="I77" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>76</v>
       </c>
@@ -2790,16 +3029,19 @@
       <c r="G78" s="3">
         <v>1</v>
       </c>
+      <c r="H78" s="3">
+        <v>2</v>
+      </c>
       <c r="I78" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>77</v>
       </c>
-      <c r="B79">
+      <c r="B79" s="4">
         <v>2</v>
       </c>
       <c r="D79" s="3">
@@ -2814,16 +3056,19 @@
       <c r="G79" s="3">
         <v>2</v>
       </c>
+      <c r="H79" s="3">
+        <v>2</v>
+      </c>
       <c r="I79" s="3">
         <f t="shared" si="1"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>78</v>
       </c>
-      <c r="B80">
+      <c r="B80" s="4">
         <v>2</v>
       </c>
       <c r="D80" s="3">
@@ -2838,16 +3083,19 @@
       <c r="G80" s="3">
         <v>2</v>
       </c>
+      <c r="H80" s="3">
+        <v>2</v>
+      </c>
       <c r="I80" s="3">
         <f t="shared" si="1"/>
-        <v>2.1147425268811282</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.0912791051825463</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>79</v>
       </c>
-      <c r="B81">
+      <c r="B81" s="4">
         <v>2</v>
       </c>
       <c r="D81" s="3">
@@ -2862,16 +3110,19 @@
       <c r="G81" s="3">
         <v>2</v>
       </c>
+      <c r="H81" s="3">
+        <v>2</v>
+      </c>
       <c r="I81" s="3">
         <f t="shared" si="1"/>
-        <v>2.0597671439071177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.0476725110792193</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>80</v>
       </c>
-      <c r="B82">
+      <c r="B82" s="4">
         <v>1</v>
       </c>
       <c r="D82" s="3">
@@ -2886,12 +3137,15 @@
       <c r="G82" s="3">
         <v>2</v>
       </c>
+      <c r="H82" s="3">
+        <v>1</v>
+      </c>
       <c r="I82" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>81</v>
       </c>
@@ -2910,12 +3164,15 @@
       <c r="G83" s="3">
         <v>3</v>
       </c>
+      <c r="H83" s="3">
+        <v>3</v>
+      </c>
       <c r="I83" s="3">
         <f t="shared" si="1"/>
-        <v>2.7831576837137408</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.825234500494767</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>82</v>
       </c>
@@ -2934,12 +3191,15 @@
       <c r="G84" s="3">
         <v>3</v>
       </c>
+      <c r="H84" s="3">
+        <v>2</v>
+      </c>
       <c r="I84" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7663237344451832</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>83</v>
       </c>
@@ -2958,16 +3218,19 @@
       <c r="G85" s="3">
         <v>3</v>
       </c>
+      <c r="H85" s="3">
+        <v>2</v>
+      </c>
       <c r="I85" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7663237344451832</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>84</v>
       </c>
-      <c r="B86">
+      <c r="B86" s="4">
         <v>2</v>
       </c>
       <c r="D86" s="3">
@@ -2982,12 +3245,15 @@
       <c r="G86" s="3">
         <v>2</v>
       </c>
+      <c r="H86" s="3">
+        <v>2</v>
+      </c>
       <c r="I86" s="3">
         <f t="shared" si="1"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>85</v>
       </c>
@@ -3006,16 +3272,19 @@
       <c r="G87" s="3">
         <v>3</v>
       </c>
+      <c r="H87" s="3">
+        <v>2</v>
+      </c>
       <c r="I87" s="3">
         <f t="shared" si="1"/>
-        <v>2.7831576837137408</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.6051710846973521</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>86</v>
       </c>
-      <c r="B88">
+      <c r="B88" s="4">
         <v>1</v>
       </c>
       <c r="D88" s="3">
@@ -3030,16 +3299,19 @@
       <c r="G88" s="3">
         <v>2</v>
       </c>
+      <c r="H88" s="3">
+        <v>1</v>
+      </c>
       <c r="I88" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>87</v>
       </c>
-      <c r="B89">
+      <c r="B89" s="4">
         <v>1</v>
       </c>
       <c r="D89" s="3">
@@ -3054,12 +3326,15 @@
       <c r="G89" s="3">
         <v>1</v>
       </c>
+      <c r="H89" s="3">
+        <v>1</v>
+      </c>
       <c r="I89" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>88</v>
       </c>
@@ -3078,12 +3353,15 @@
       <c r="G90" s="3">
         <v>2</v>
       </c>
+      <c r="H90" s="3">
+        <v>1</v>
+      </c>
       <c r="I90" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>89</v>
       </c>
@@ -3102,16 +3380,19 @@
       <c r="G91" s="3">
         <v>2</v>
       </c>
+      <c r="H91" s="3">
+        <v>2</v>
+      </c>
       <c r="I91" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.515716566510398</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>90</v>
       </c>
-      <c r="B92">
+      <c r="B92" s="4">
         <v>3</v>
       </c>
       <c r="D92" s="3">
@@ -3126,12 +3407,15 @@
       <c r="G92" s="3">
         <v>3</v>
       </c>
+      <c r="H92" s="3">
+        <v>2</v>
+      </c>
       <c r="I92" s="3">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7663237344451832</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>91</v>
       </c>
@@ -3150,12 +3434,15 @@
       <c r="G93" s="3">
         <v>2</v>
       </c>
+      <c r="H93" s="3">
+        <v>2</v>
+      </c>
       <c r="I93" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>92</v>
       </c>
@@ -3174,16 +3461,19 @@
       <c r="G94" s="3">
         <v>2</v>
       </c>
+      <c r="H94" s="3">
+        <v>1</v>
+      </c>
       <c r="I94" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4309690811052556</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>93</v>
       </c>
-      <c r="B95">
+      <c r="B95" s="4">
         <v>2</v>
       </c>
       <c r="D95" s="3">
@@ -3198,12 +3488,15 @@
       <c r="G95" s="3">
         <v>2</v>
       </c>
+      <c r="H95" s="3">
+        <v>2</v>
+      </c>
       <c r="I95" s="3">
         <f t="shared" si="1"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -3222,16 +3515,19 @@
       <c r="G96" s="3">
         <v>3</v>
       </c>
+      <c r="H96" s="3">
+        <v>1</v>
+      </c>
       <c r="I96" s="3">
         <f t="shared" si="1"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>95</v>
       </c>
-      <c r="B97">
+      <c r="B97" s="4">
         <v>1</v>
       </c>
       <c r="D97" s="3">
@@ -3246,16 +3542,19 @@
       <c r="G97" s="3">
         <v>2</v>
       </c>
+      <c r="H97" s="3">
+        <v>1</v>
+      </c>
       <c r="I97" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4309690811052556</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>96</v>
       </c>
-      <c r="B98">
+      <c r="B98" s="4">
         <v>2</v>
       </c>
       <c r="D98" s="3">
@@ -3270,12 +3569,15 @@
       <c r="G98" s="3">
         <v>2</v>
       </c>
+      <c r="H98" s="3">
+        <v>2</v>
+      </c>
       <c r="I98" s="3">
         <f t="shared" si="1"/>
-        <v>2.2133638394006434</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.1689435423953971</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -3294,16 +3596,19 @@
       <c r="G99" s="3">
         <v>3</v>
       </c>
+      <c r="H99" s="3">
+        <v>2</v>
+      </c>
       <c r="I99" s="3">
         <f t="shared" si="1"/>
-        <v>2.9129506302439405</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.7019200770412271</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>98</v>
       </c>
-      <c r="B100">
+      <c r="B100" s="4">
         <v>2</v>
       </c>
       <c r="D100" s="3">
@@ -3318,16 +3623,19 @@
       <c r="G100" s="3">
         <v>2</v>
       </c>
+      <c r="H100" s="3">
+        <v>2</v>
+      </c>
       <c r="I100" s="3">
         <f t="shared" si="1"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>99</v>
       </c>
-      <c r="B101">
+      <c r="B101" s="4">
         <v>2</v>
       </c>
       <c r="D101" s="3">
@@ -3342,16 +3650,19 @@
       <c r="G101" s="3">
         <v>2</v>
       </c>
+      <c r="H101" s="3">
+        <v>2</v>
+      </c>
       <c r="I101" s="3">
         <f t="shared" si="1"/>
-        <v>1.681792830507429</v>
-      </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.7411011265922482</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>100</v>
       </c>
-      <c r="B102">
+      <c r="B102" s="4">
         <v>1</v>
       </c>
       <c r="D102" s="3">
@@ -3366,16 +3677,19 @@
       <c r="G102" s="3">
         <v>1</v>
       </c>
+      <c r="H102" s="3">
+        <v>1</v>
+      </c>
       <c r="I102" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>101</v>
       </c>
-      <c r="B103">
+      <c r="B103" s="4">
         <v>1</v>
       </c>
       <c r="D103" s="3">
@@ -3390,12 +3704,15 @@
       <c r="G103" s="3">
         <v>2</v>
       </c>
+      <c r="H103" s="3">
+        <v>2</v>
+      </c>
       <c r="I103" s="3">
         <f t="shared" si="1"/>
-        <v>1.3160740129524926</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4309690811052556</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>102</v>
       </c>
@@ -3414,12 +3731,15 @@
       <c r="G104" s="3">
         <v>1</v>
       </c>
+      <c r="H104" s="3">
+        <v>1</v>
+      </c>
       <c r="I104" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>103</v>
       </c>
@@ -3438,16 +3758,19 @@
       <c r="G105" s="3">
         <v>2</v>
       </c>
+      <c r="H105" s="3">
+        <v>2</v>
+      </c>
       <c r="I105" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>104</v>
       </c>
-      <c r="B106">
+      <c r="B106" s="4">
         <v>2</v>
       </c>
       <c r="D106" s="3">
@@ -3462,16 +3785,19 @@
       <c r="G106" s="3">
         <v>3</v>
       </c>
+      <c r="H106" s="3">
+        <v>2</v>
+      </c>
       <c r="I106" s="3">
         <f t="shared" si="1"/>
-        <v>2.2795070569547775</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.22064303492292</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>105</v>
       </c>
-      <c r="B107">
+      <c r="B107" s="4">
         <v>1</v>
       </c>
       <c r="D107" s="3">
@@ -3486,16 +3812,19 @@
       <c r="G107" s="3">
         <v>2</v>
       </c>
+      <c r="H107" s="3">
+        <v>1</v>
+      </c>
       <c r="I107" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>106</v>
       </c>
-      <c r="B108">
+      <c r="B108" s="4">
         <v>1</v>
       </c>
       <c r="D108" s="3">
@@ -3510,16 +3839,19 @@
       <c r="G108" s="3">
         <v>2</v>
       </c>
+      <c r="H108" s="3">
+        <v>1</v>
+      </c>
       <c r="I108" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>107</v>
       </c>
-      <c r="B109">
+      <c r="B109" s="4">
         <v>2</v>
       </c>
       <c r="D109" s="3">
@@ -3534,12 +3866,15 @@
       <c r="G109" s="3">
         <v>1</v>
       </c>
+      <c r="H109" s="3">
+        <v>2</v>
+      </c>
       <c r="I109" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>108</v>
       </c>
@@ -3558,12 +3893,15 @@
       <c r="G110" s="3">
         <v>2</v>
       </c>
+      <c r="H110" s="3">
+        <v>1</v>
+      </c>
       <c r="I110" s="3">
         <f t="shared" si="1"/>
-        <v>1.4142135623730949</v>
-      </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.3195079107728942</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>109</v>
       </c>
@@ -3582,16 +3920,19 @@
       <c r="G111" s="3">
         <v>3</v>
       </c>
+      <c r="H111" s="3">
+        <v>2</v>
+      </c>
       <c r="I111" s="3">
         <f t="shared" si="1"/>
-        <v>2.7108060108295344</v>
-      </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.5508490012515819</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>110</v>
       </c>
-      <c r="B112">
+      <c r="B112" s="4">
         <v>2</v>
       </c>
       <c r="D112" s="3">
@@ -3606,16 +3947,19 @@
       <c r="G112" s="3">
         <v>2</v>
       </c>
+      <c r="H112" s="3">
+        <v>2</v>
+      </c>
       <c r="I112" s="3">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>111</v>
       </c>
-      <c r="B113">
+      <c r="B113" s="4">
         <v>2</v>
       </c>
       <c r="D113" s="3">
@@ -3630,16 +3974,19 @@
       <c r="G113" s="3">
         <v>2</v>
       </c>
+      <c r="H113" s="3">
+        <v>2</v>
+      </c>
       <c r="I113" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>112</v>
       </c>
-      <c r="B114">
+      <c r="B114" s="4">
         <v>1</v>
       </c>
       <c r="D114" s="3">
@@ -3654,16 +4001,19 @@
       <c r="G114" s="3">
         <v>1</v>
       </c>
+      <c r="H114" s="3">
+        <v>2</v>
+      </c>
       <c r="I114" s="3">
         <f t="shared" si="1"/>
-        <v>1.3160740129524926</v>
-      </c>
-    </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.4309690811052556</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>113</v>
       </c>
-      <c r="B115">
+      <c r="B115" s="4">
         <v>2</v>
       </c>
       <c r="D115" s="3">
@@ -3678,12 +4028,15 @@
       <c r="G115" s="3">
         <v>2</v>
       </c>
+      <c r="H115" s="3">
+        <v>2</v>
+      </c>
       <c r="I115" s="3">
         <f t="shared" si="1"/>
-        <v>1.8612097182041991</v>
-      </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.8881750225898042</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>114</v>
       </c>
@@ -3702,16 +4055,19 @@
       <c r="G116" s="3">
         <v>2</v>
       </c>
+      <c r="H116" s="3">
+        <v>2</v>
+      </c>
       <c r="I116" s="3">
         <f t="shared" si="1"/>
-        <v>1.681792830507429</v>
-      </c>
-    </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.7411011265922482</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>115</v>
       </c>
-      <c r="B117">
+      <c r="B117" s="4">
         <v>1</v>
       </c>
       <c r="D117" s="3">
@@ -3726,16 +4082,19 @@
       <c r="G117" s="3">
         <v>1</v>
       </c>
+      <c r="H117" s="3">
+        <v>1</v>
+      </c>
       <c r="I117" s="3">
         <f t="shared" si="1"/>
-        <v>1.3160740129524926</v>
-      </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.2457309396155174</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>116</v>
       </c>
-      <c r="B118">
+      <c r="B118" s="4">
         <v>1</v>
       </c>
       <c r="D118" s="3">
@@ -3750,16 +4109,19 @@
       <c r="G118" s="3">
         <v>2</v>
       </c>
+      <c r="H118" s="3">
+        <v>1</v>
+      </c>
       <c r="I118" s="3">
         <f t="shared" si="1"/>
-        <v>1.189207115002721</v>
-      </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.1486983549970351</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>117</v>
       </c>
-      <c r="B119">
+      <c r="B119" s="4">
         <v>2</v>
       </c>
       <c r="D119" s="3">
@@ -3774,16 +4136,19 @@
       <c r="G119" s="3">
         <v>1</v>
       </c>
+      <c r="H119" s="3">
+        <v>2</v>
+      </c>
       <c r="I119" s="3">
         <f t="shared" si="1"/>
-        <v>1.5650845800732873</v>
-      </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.6437518295172258</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>118</v>
       </c>
-      <c r="B120">
+      <c r="B120" s="4">
         <v>1</v>
       </c>
       <c r="D120" s="3">
@@ -3798,16 +4163,19 @@
       <c r="G120" s="3">
         <v>1</v>
       </c>
+      <c r="H120" s="3">
+        <v>1</v>
+      </c>
       <c r="I120" s="3">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>119</v>
       </c>
-      <c r="B121">
+      <c r="B121" s="4">
         <v>3</v>
       </c>
       <c r="D121" s="3">
@@ -3822,16 +4190,19 @@
       <c r="G121" s="3">
         <v>3</v>
       </c>
+      <c r="H121" s="3">
+        <v>2</v>
+      </c>
       <c r="I121" s="3">
         <f t="shared" si="1"/>
-        <v>3.0800702882410231</v>
-      </c>
-    </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2.825234500494767</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>120</v>
       </c>
-      <c r="B122">
+      <c r="B122" s="4">
         <v>2</v>
       </c>
       <c r="D122" s="3">
@@ -3846,16 +4217,19 @@
       <c r="G122" s="3">
         <v>2</v>
       </c>
+      <c r="H122" s="3">
+        <v>2</v>
+      </c>
       <c r="I122" s="3">
         <f t="shared" si="1"/>
-        <v>1.681792830507429</v>
-      </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+        <v>1.7411011265922482</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>121</v>
       </c>
-      <c r="B123">
+      <c r="B123" s="4">
         <v>2</v>
       </c>
       <c r="D123" s="3">
@@ -3870,9 +4244,12 @@
       <c r="G123" s="3">
         <v>3</v>
       </c>
+      <c r="H123" s="3">
+        <v>2</v>
+      </c>
       <c r="I123" s="3">
         <f t="shared" si="1"/>
-        <v>2.4494897427831779</v>
+        <v>2.3521580450493471</v>
       </c>
     </row>
   </sheetData>

</xml_diff>